<commit_message>
feat: Introduce new data files, database migrations for invoicing and portfolio, and various processing scripts, alongside updates to existing data and core logic.
</commit_message>
<xml_diff>
--- a/Shared/Sources/excel_data/Copy of Huisvestingslijst December 2025.xlsx
+++ b/Shared/Sources/excel_data/Copy of Huisvestingslijst December 2025.xlsx
@@ -30291,19 +30291,19 @@
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="cd1a0b34-7396-4131-ae27-ed7b12d16f43">
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="7e7f2dcd-0c2b-4478-ad05-247cf739c5b2">
       <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="7ffa2fad-f732-4a38-9c4b-50be636d4d5f" xsi:nil="true"/>
+    <TaxCatchAll xmlns="7c6541c9-858d-46cc-aee4-1fa681dc1bd6" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101003F5C5B848C0E1B4CBCD71E486F17F49A" ma:contentTypeVersion="12" ma:contentTypeDescription="Een nieuw document maken." ma:contentTypeScope="" ma:versionID="4b6117036416fcb033143a080870dac3">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="cd1a0b34-7396-4131-ae27-ed7b12d16f43" xmlns:ns3="7ffa2fad-f732-4a38-9c4b-50be636d4d5f" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="d7363b7df22250cb37e6093ec83bb850" ns2:_="" ns3:_="">
-    <xsd:import namespace="cd1a0b34-7396-4131-ae27-ed7b12d16f43"/>
-    <xsd:import namespace="7ffa2fad-f732-4a38-9c4b-50be636d4d5f"/>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100FD8216A3BCF59A4CAC1EDC9B65F03F94" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d0e72e358fff385e948993b5140718f2">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="7e7f2dcd-0c2b-4478-ad05-247cf739c5b2" xmlns:ns3="7c6541c9-858d-46cc-aee4-1fa681dc1bd6" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f2e1edef662b1e8a4a57019bf45cf5f9" ns2:_="" ns3:_="">
+    <xsd:import namespace="7e7f2dcd-0c2b-4478-ad05-247cf739c5b2"/>
+    <xsd:import namespace="7c6541c9-858d-46cc-aee4-1fa681dc1bd6"/>
     <xsd:element name="properties">
       <xsd:complexType>
         <xsd:sequence>
@@ -30312,15 +30312,18 @@
               <xsd:all>
                 <xsd:element ref="ns2:MediaServiceMetadata" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceFastMetadata" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceSearchProperties" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceDateTaken" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceLocation" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceGenerationTime" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceEventHashCode" minOccurs="0"/>
                 <xsd:element ref="ns2:lcf76f155ced4ddcb4097134ff3c332f" minOccurs="0"/>
                 <xsd:element ref="ns3:TaxCatchAll" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceOCR" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceGenerationTime" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceEventHashCode" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceLocation" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaLengthInSeconds" minOccurs="0"/>
+                <xsd:element ref="ns3:SharedWithUsers" minOccurs="0"/>
+                <xsd:element ref="ns3:SharedWithDetails" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceObjectDetectorVersions" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceSearchProperties" minOccurs="0"/>
               </xsd:all>
             </xsd:complexType>
           </xsd:element>
@@ -30328,7 +30331,7 @@
       </xsd:complexType>
     </xsd:element>
   </xsd:schema>
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="cd1a0b34-7396-4131-ae27-ed7b12d16f43" elementFormDefault="qualified">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="7e7f2dcd-0c2b-4478-ad05-247cf739c5b2" elementFormDefault="qualified">
     <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <xsd:element name="MediaServiceMetadata" ma:index="8" nillable="true" ma:displayName="MediaServiceMetadata" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
@@ -30341,55 +30344,60 @@
         <xsd:restriction base="dms:Note"/>
       </xsd:simpleType>
     </xsd:element>
-    <xsd:element name="MediaServiceSearchProperties" ma:index="10" nillable="true" ma:displayName="MediaServiceSearchProperties" ma:hidden="true" ma:internalName="MediaServiceSearchProperties" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceDateTaken" ma:index="11" nillable="true" ma:displayName="MediaServiceDateTaken" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
+    <xsd:element name="MediaServiceDateTaken" ma:index="10" nillable="true" ma:displayName="MediaServiceDateTaken" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Text"/>
       </xsd:simpleType>
     </xsd:element>
-    <xsd:element name="lcf76f155ced4ddcb4097134ff3c332f" ma:index="13" nillable="true" ma:taxonomy="true" ma:internalName="lcf76f155ced4ddcb4097134ff3c332f" ma:taxonomyFieldName="MediaServiceImageTags" ma:displayName="Afbeeldingtags" ma:readOnly="false" ma:fieldId="{5cf76f15-5ced-4ddc-b409-7134ff3c332f}" ma:taxonomyMulti="true" ma:sspId="5f29922b-bc8b-44be-bee2-c343b708f3d5" ma:termSetId="09814cd3-568e-fe90-9814-8d621ff8fb84" ma:anchorId="fba54fb3-c3e1-fe81-a776-ca4b69148c4d" ma:open="true" ma:isKeyword="false">
+    <xsd:element name="MediaServiceLocation" ma:index="11" nillable="true" ma:displayName="Location" ma:indexed="true" ma:internalName="MediaServiceLocation" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceGenerationTime" ma:index="12" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceEventHashCode" ma:index="13" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="lcf76f155ced4ddcb4097134ff3c332f" ma:index="15" nillable="true" ma:taxonomy="true" ma:internalName="lcf76f155ced4ddcb4097134ff3c332f" ma:taxonomyFieldName="MediaServiceImageTags" ma:displayName="Image Tags" ma:readOnly="false" ma:fieldId="{5cf76f15-5ced-4ddc-b409-7134ff3c332f}" ma:taxonomyMulti="true" ma:sspId="5bd66242-e0b1-4d5e-a424-ed2be647a714" ma:termSetId="09814cd3-568e-fe90-9814-8d621ff8fb84" ma:anchorId="fba54fb3-c3e1-fe81-a776-ca4b69148c4d" ma:open="true" ma:isKeyword="false">
       <xsd:complexType>
         <xsd:sequence>
           <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
         </xsd:sequence>
       </xsd:complexType>
     </xsd:element>
-    <xsd:element name="MediaServiceOCR" ma:index="15" nillable="true" ma:displayName="Extracted Text" ma:internalName="MediaServiceOCR" ma:readOnly="true">
+    <xsd:element name="MediaServiceOCR" ma:index="17" nillable="true" ma:displayName="Extracted Text" ma:internalName="MediaServiceOCR" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Note">
           <xsd:maxLength value="255"/>
         </xsd:restriction>
       </xsd:simpleType>
     </xsd:element>
-    <xsd:element name="MediaServiceGenerationTime" ma:index="16" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
+    <xsd:element name="MediaLengthInSeconds" ma:index="18" nillable="true" ma:displayName="MediaLengthInSeconds" ma:hidden="true" ma:internalName="MediaLengthInSeconds" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Unknown"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceObjectDetectorVersions" ma:index="21" nillable="true" ma:displayName="MediaServiceObjectDetectorVersions" ma:description="" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceObjectDetectorVersions" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Text"/>
       </xsd:simpleType>
     </xsd:element>
-    <xsd:element name="MediaServiceEventHashCode" ma:index="17" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
+    <xsd:element name="MediaServiceSearchProperties" ma:index="22" nillable="true" ma:displayName="MediaServiceSearchProperties" ma:hidden="true" ma:internalName="MediaServiceSearchProperties" ma:readOnly="true">
       <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceLocation" ma:index="18" nillable="true" ma:displayName="Location" ma:indexed="true" ma:internalName="MediaServiceLocation" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaLengthInSeconds" ma:index="19" nillable="true" ma:displayName="MediaLengthInSeconds" ma:hidden="true" ma:internalName="MediaLengthInSeconds" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Unknown"/>
+        <xsd:restriction base="dms:Note"/>
       </xsd:simpleType>
     </xsd:element>
   </xsd:schema>
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="7ffa2fad-f732-4a38-9c4b-50be636d4d5f" elementFormDefault="qualified">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="7c6541c9-858d-46cc-aee4-1fa681dc1bd6" elementFormDefault="qualified">
     <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <xsd:element name="TaxCatchAll" ma:index="14" nillable="true" ma:displayName="Taxonomy Catch All Column" ma:hidden="true" ma:list="{86c5d5e6-dfbe-467e-81d2-b56045a2c173}" ma:internalName="TaxCatchAll" ma:showField="CatchAllData" ma:web="7ffa2fad-f732-4a38-9c4b-50be636d4d5f">
+    <xsd:element name="TaxCatchAll" ma:index="16" nillable="true" ma:displayName="Taxonomy Catch All Column" ma:hidden="true" ma:list="{5de6d577-5e06-4df3-9e53-a11405c55b7c}" ma:internalName="TaxCatchAll" ma:showField="CatchAllData" ma:web="7c6541c9-858d-46cc-aee4-1fa681dc1bd6">
       <xsd:complexType>
         <xsd:complexContent>
           <xsd:extension base="dms:MultiChoiceLookup">
@@ -30399,6 +30407,32 @@
           </xsd:extension>
         </xsd:complexContent>
       </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="SharedWithUsers" ma:index="19" nillable="true" ma:displayName="Shared With" ma:internalName="SharedWithUsers" ma:readOnly="true">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:UserMulti">
+            <xsd:sequence>
+              <xsd:element name="UserInfo" minOccurs="0" maxOccurs="unbounded">
+                <xsd:complexType>
+                  <xsd:sequence>
+                    <xsd:element name="DisplayName" type="xsd:string" minOccurs="0"/>
+                    <xsd:element name="AccountId" type="dms:UserId" minOccurs="0" nillable="true"/>
+                    <xsd:element name="AccountType" type="xsd:string" minOccurs="0"/>
+                  </xsd:sequence>
+                </xsd:complexType>
+              </xsd:element>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="SharedWithDetails" ma:index="20" nillable="true" ma:displayName="Shared With Details" ma:internalName="SharedWithDetails" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
     </xsd:element>
   </xsd:schema>
   <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
@@ -30410,8 +30444,8 @@
         <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
         <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
         <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Inhoudstype"/>
-        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Titel"/>
+        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Content Type"/>
+        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Title"/>
         <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
         <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
         <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
@@ -30528,20 +30562,5 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2030D7AC-A5D8-4D2D-BD61-EE4F1CD14A29}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="cd1a0b34-7396-4131-ae27-ed7b12d16f43"/>
-    <ds:schemaRef ds:uri="7ffa2fad-f732-4a38-9c4b-50be636d4d5f"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{16F42EF8-0EB0-413C-B4BF-8FD1B2E8CE96}"/>
 </file>
</xml_diff>